<commit_message>
website title update from React App to kanjitest
</commit_message>
<xml_diff>
--- a/backend/exports/202311.xlsx
+++ b/backend/exports/202311.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -766,9 +766,20 @@
         <v>00:25</v>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>202474</v>
+      </c>
+      <c r="B34" t="str">
+        <v>100/100</v>
+      </c>
+      <c r="C34" t="str">
+        <v>03:14</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C33"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C34"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>